<commit_message>
Added the final presentation, and a schematic of the Main board
</commit_message>
<xml_diff>
--- a/Design/Statics.xlsx
+++ b/Design/Statics.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="480" yWindow="30" windowWidth="20610" windowHeight="11640"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>I</t>
   </si>
@@ -65,6 +66,12 @@
   </si>
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>Modulus</t>
+  </si>
+  <si>
+    <t>Max PSI</t>
   </si>
 </sst>
 </file>
@@ -164,12 +171,12 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$6:$F$20</c:f>
+              <c:f>'Sheet1 (2)'!$F$6:$F$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>3.4947916666666665</c:v>
+                  <c:v>107.03645833333331</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.984049479166667</c:v>
@@ -218,12 +225,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$6:$G$20</c:f>
+              <c:f>'Sheet1 (2)'!$G$6:$G$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2.75</c:v>
+                  <c:v>7.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.4375</c:v>
@@ -280,11 +287,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="183139328"/>
-        <c:axId val="183159040"/>
+        <c:axId val="48125824"/>
+        <c:axId val="48127360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="183139328"/>
+        <c:axId val="48125824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -294,12 +301,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183159040"/>
+        <c:crossAx val="48127360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="183159040"/>
+        <c:axId val="48127360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -310,7 +317,205 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183139328"/>
+        <c:crossAx val="48125824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$6:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>3.4947916666666665</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.984049479166667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3288413866666673</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0169107200000012</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.55782874589866704</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0677083333333339</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.9150390625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5991987200000022</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9813427200000007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.338541666666664</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.06719970703125</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.8615133866666724</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.2086067200000059</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.8251613538986717</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$6:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93440000000000012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70560000000000045</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3799039999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0944000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.82560000000000144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.234375</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.4144000000000005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0655999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.57190399999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="148569088"/>
+        <c:axId val="149095168"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="148569088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="149095168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="149095168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="148569088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -333,6 +538,43 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -654,10 +896,1048 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:R22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>18</v>
+      </c>
+      <c r="R5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E6">
+        <f>(B6*C6^3)/12</f>
+        <v>500</v>
+      </c>
+      <c r="F6">
+        <f>E6-(((B6-(D6*2))*(C6-(D6*2))^3)/12)</f>
+        <v>107.03645833333331</v>
+      </c>
+      <c r="G6">
+        <f>(B6*C6)-((B6-(D6*2))*(C6-(D6*2)))</f>
+        <v>7.75</v>
+      </c>
+      <c r="H6" s="2">
+        <v>48</v>
+      </c>
+      <c r="I6" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K6" s="4">
+        <f>(I6*(H6^3))/(48*J6*F6)</f>
+        <v>0.136995916093263</v>
+      </c>
+      <c r="L6">
+        <f>I6/2*H6/2</f>
+        <v>144000</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ref="N6:N19" si="0">H6*C6*B6*M6</f>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>C6/2</f>
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <f>(L6*O6)/F6</f>
+        <v>6726.6799669115871</v>
+      </c>
+      <c r="Q6">
+        <v>7250</v>
+      </c>
+      <c r="R6" s="5">
+        <f>(P6/Q6)</f>
+        <v>0.92781792647056371</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>0.125</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E21" si="1">(B7*C7^3)/12</f>
+        <v>6.75</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7:F21" si="2">E7-(((B7-(D7*2))*(C7-(D7*2))^3)/12)</f>
+        <v>1.984049479166667</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G21" si="3">(B7*C7)-((B7-(D7*2))*(C7-(D7*2)))</f>
+        <v>1.4375</v>
+      </c>
+      <c r="H7" s="2">
+        <v>20</v>
+      </c>
+      <c r="I7" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" ref="K7:K21" si="4">(I7*(H7^3))/(48*J7*F7)</f>
+        <v>0.53462975716902261</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ref="L7:L21" si="5">I7/2*H7/2</f>
+        <v>60000</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ref="O7:O21" si="6">C7/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="P7">
+        <f t="shared" ref="P7:P21" si="7">(L7*O7)/F7</f>
+        <v>45361.771944216562</v>
+      </c>
+      <c r="Q7">
+        <v>7250</v>
+      </c>
+      <c r="R7" s="5">
+        <f t="shared" ref="R7:R21" si="8">(P7/Q7)</f>
+        <v>6.2567961302367667</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>0.08</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>6.75</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>1.3288413866666673</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>0.93440000000000012</v>
+      </c>
+      <c r="H8" s="2">
+        <v>20</v>
+      </c>
+      <c r="I8" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="4"/>
+        <v>0.79823815084431882</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="5"/>
+        <v>60000</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="6"/>
+        <v>1.5</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="7"/>
+        <v>67728.173507419531</v>
+      </c>
+      <c r="Q8">
+        <v>7250</v>
+      </c>
+      <c r="R8" s="5">
+        <f t="shared" si="8"/>
+        <v>9.3418170355061427</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>0.06</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>6.75</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>1.0169107200000012</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>0.70560000000000045</v>
+      </c>
+      <c r="H9" s="2">
+        <v>20</v>
+      </c>
+      <c r="I9" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K9" s="4">
+        <f t="shared" si="4"/>
+        <v>1.0430924469536518</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="5"/>
+        <v>60000</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="6"/>
+        <v>1.5</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="7"/>
+        <v>88503.344718403503</v>
+      </c>
+      <c r="Q9">
+        <v>7250</v>
+      </c>
+      <c r="R9" s="5">
+        <f t="shared" si="8"/>
+        <v>12.207357892193587</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>6.75</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>0.55782874589866704</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>0.3799039999999998</v>
+      </c>
+      <c r="H10" s="2">
+        <v>20</v>
+      </c>
+      <c r="I10" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K10" s="4">
+        <f t="shared" si="4"/>
+        <v>1.9015368050804777</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="5"/>
+        <v>60000</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="6"/>
+        <v>1.5</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="7"/>
+        <v>161339.83890523462</v>
+      </c>
+      <c r="Q10">
+        <v>7250</v>
+      </c>
+      <c r="R10" s="5">
+        <f t="shared" si="8"/>
+        <v>22.253770883480637</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>7.0677083333333339</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>3.25</v>
+      </c>
+      <c r="H11" s="2">
+        <v>20</v>
+      </c>
+      <c r="I11" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K11" s="4">
+        <f t="shared" si="4"/>
+        <v>0.1500814466629142</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="5"/>
+        <v>60000</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="7"/>
+        <v>16978.629329403095</v>
+      </c>
+      <c r="Q11">
+        <v>7250</v>
+      </c>
+      <c r="R11" s="5">
+        <f t="shared" si="8"/>
+        <v>2.3418799075038752</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>0.125</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>3.9150390625</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>1.6875</v>
+      </c>
+      <c r="H12" s="2">
+        <v>20</v>
+      </c>
+      <c r="I12" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K12" s="4">
+        <f t="shared" si="4"/>
+        <v>0.27093775421511546</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="5"/>
+        <v>60000</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="7"/>
+        <v>30651.035170865551</v>
+      </c>
+      <c r="Q12">
+        <v>7250</v>
+      </c>
+      <c r="R12" s="5">
+        <f t="shared" si="8"/>
+        <v>4.2277289890849037</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>0.08</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>2.5991987200000022</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>1.0944000000000003</v>
+      </c>
+      <c r="H13" s="2">
+        <v>20</v>
+      </c>
+      <c r="I13" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" si="4"/>
+        <v>0.4080995743404337</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="5"/>
+        <v>60000</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="7"/>
+        <v>46168.07444411172</v>
+      </c>
+      <c r="Q13">
+        <v>7250</v>
+      </c>
+      <c r="R13" s="5">
+        <f t="shared" si="8"/>
+        <v>6.3680102681533404</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>0.06</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>1.9813427200000007</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>0.82560000000000144</v>
+      </c>
+      <c r="H14" s="2">
+        <v>20</v>
+      </c>
+      <c r="I14" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.53536012752917417</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="5"/>
+        <v>60000</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="7"/>
+        <v>60564.988978787049</v>
+      </c>
+      <c r="Q14">
+        <v>7250</v>
+      </c>
+      <c r="R14" s="5">
+        <f t="shared" si="8"/>
+        <v>8.353791583280973</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>19.338541666666664</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>4.25</v>
+      </c>
+      <c r="H15" s="2">
+        <v>20</v>
+      </c>
+      <c r="I15" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" si="4"/>
+        <v>5.4850666070986973E-2</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="5"/>
+        <v>60000</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="7"/>
+        <v>9307.8373283059536</v>
+      </c>
+      <c r="Q15">
+        <v>7250</v>
+      </c>
+      <c r="R15" s="5">
+        <f t="shared" si="8"/>
+        <v>1.2838396314904763</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>0.1875</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>15.06719970703125</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>3.234375</v>
+      </c>
+      <c r="H16" s="2">
+        <v>20</v>
+      </c>
+      <c r="I16" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J16" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K16" s="4">
+        <f t="shared" si="4"/>
+        <v>7.0400068485400147E-2</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="5"/>
+        <v>60000</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="7"/>
+        <v>11946.480002916622</v>
+      </c>
+      <c r="Q16">
+        <v>7250</v>
+      </c>
+      <c r="R16" s="5">
+        <f t="shared" si="8"/>
+        <v>1.6477903452298788</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>0.08</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>6.8615133866666724</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>1.4144000000000005</v>
+      </c>
+      <c r="H17" s="2">
+        <v>20</v>
+      </c>
+      <c r="I17" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K17" s="4">
+        <f t="shared" si="4"/>
+        <v>0.15459153563985178</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="5"/>
+        <v>60000</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="7"/>
+        <v>26233.279723650605</v>
+      </c>
+      <c r="Q17">
+        <v>7250</v>
+      </c>
+      <c r="R17" s="5">
+        <f t="shared" si="8"/>
+        <v>3.618383410158704</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>0.06</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>5.2086067200000059</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>1.0655999999999999</v>
+      </c>
+      <c r="H18" s="2">
+        <v>20</v>
+      </c>
+      <c r="I18" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K18" s="4">
+        <f t="shared" si="4"/>
+        <v>0.20364983349293836</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="5"/>
+        <v>60000</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="7"/>
+        <v>34558.186032521146</v>
+      </c>
+      <c r="Q18">
+        <v>7250</v>
+      </c>
+      <c r="R18" s="5">
+        <f t="shared" si="8"/>
+        <v>4.7666463493132616</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>2.8251613538986717</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>0.57190399999999997</v>
+      </c>
+      <c r="H19" s="2">
+        <v>20</v>
+      </c>
+      <c r="I19" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K19" s="4">
+        <f t="shared" si="4"/>
+        <v>0.37545887062146388</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="5"/>
+        <v>60000</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="7"/>
+        <v>63713.175090549514</v>
+      </c>
+      <c r="Q19">
+        <v>7250</v>
+      </c>
+      <c r="R19" s="5">
+        <f t="shared" si="8"/>
+        <v>8.7880241504206218</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>0.5</v>
+      </c>
+      <c r="D20">
+        <v>0.25</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="H20" s="2">
+        <v>9</v>
+      </c>
+      <c r="I20" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J20" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K20" s="4">
+        <f t="shared" si="4"/>
+        <v>0.77327354872722853</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="5"/>
+        <v>27000</v>
+      </c>
+      <c r="M20">
+        <v>9.7543000000000005E-2</v>
+      </c>
+      <c r="N20">
+        <f>H20*C20*B20*M20</f>
+        <v>5.2673220000000001</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="6"/>
+        <v>0.25</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="7"/>
+        <v>54000</v>
+      </c>
+      <c r="Q20">
+        <v>7250</v>
+      </c>
+      <c r="R20" s="5">
+        <f t="shared" si="8"/>
+        <v>7.4482758620689653</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="H21" s="2">
+        <v>20</v>
+      </c>
+      <c r="I21" s="3">
+        <v>12000</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1885490.5904900001</v>
+      </c>
+      <c r="K21" s="4">
+        <f t="shared" si="4"/>
+        <v>1.0607318912582011</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="5"/>
+        <v>60000</v>
+      </c>
+      <c r="M21">
+        <v>9.7543000000000005E-2</v>
+      </c>
+      <c r="N21">
+        <f>H21*C21*B21*M21</f>
+        <v>23.410320000000002</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="7"/>
+        <v>30000</v>
+      </c>
+      <c r="Q21">
+        <v>7250</v>
+      </c>
+      <c r="R21" s="5">
+        <f t="shared" si="8"/>
+        <v>4.1379310344827589</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H22" s="2"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>